<commit_message>
1.Code:convertXlsToJSON.py changed cols 2.Data:xls NewDraft colsNeeded 3.Img:db structure pic
</commit_message>
<xml_diff>
--- a/Data/project2_columns_needed.xlsx
+++ b/Data/project2_columns_needed.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\supri\Documents\Web-Health-Index\Web-Health-Index\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project2Sep11\Web-Health-Index\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45B39474-8C9C-46F7-B0E4-23DF21542836}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9384EE62-82DF-4D1C-B53A-DAE918F0E0AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7260" xr2:uid="{31870007-FE29-4677-A5B4-324CC5A5B87A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Attributes" sheetId="2" r:id="rId1"/>
-    <sheet name="Draft 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Draft 3" sheetId="3" r:id="rId1"/>
+    <sheet name="Draft 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Draft 1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
   <si>
     <t>Premature death</t>
   </si>
@@ -91,25 +92,187 @@
     <t>Health Behaviours</t>
   </si>
   <si>
+    <t xml:space="preserve">Tobacco </t>
+  </si>
+  <si>
+    <t>Diet and Exercise</t>
+  </si>
+  <si>
+    <t>Alchol &amp; drug</t>
+  </si>
+  <si>
     <t>Clinical Care</t>
   </si>
   <si>
+    <t>Access to care</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
     <t>Economic Factors</t>
   </si>
   <si>
+    <t>Empl</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
     <t>Physical Environment</t>
   </si>
   <si>
+    <t>Air and water Quality</t>
+  </si>
+  <si>
+    <t>Housing and Transit</t>
+  </si>
+  <si>
+    <t>Mamography</t>
+  </si>
+  <si>
+    <t>% Smokers</t>
+  </si>
+  <si>
+    <t>Food Environment Index</t>
+  </si>
+  <si>
+    <t>Access to exercise opportunities</t>
+  </si>
+  <si>
+    <t>Driving Deaths</t>
+  </si>
+  <si>
+    <t>Uninsured</t>
+  </si>
+  <si>
+    <t>Primary Care Physicians</t>
+  </si>
+  <si>
+    <t>Graduation Rate</t>
+  </si>
+  <si>
+    <t>% Unemployed</t>
+  </si>
+  <si>
+    <t>80th Percentile Income</t>
+  </si>
+  <si>
+    <t>Air pollution - particulate matter</t>
+  </si>
+  <si>
+    <t>Average Daily PM2.5</t>
+  </si>
+  <si>
+    <t>Households with Severe Problems</t>
+  </si>
+  <si>
+    <t>Drinking water violations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presence of violation </t>
+  </si>
+  <si>
+    <t>Z-Score of Drinking water violations</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>Preventive Medicare</t>
+  </si>
+  <si>
+    <t>BK</t>
+  </si>
+  <si>
+    <t>BP</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>AJ</t>
+  </si>
+  <si>
+    <t>AW</t>
+  </si>
+  <si>
+    <t>CX</t>
+  </si>
+  <si>
+    <t>DH</t>
+  </si>
+  <si>
+    <t>DQ</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>EO</t>
+  </si>
+  <si>
+    <t>EP</t>
+  </si>
+  <si>
+    <t>Cell Value</t>
+  </si>
+  <si>
+    <t>Columns Needed</t>
+  </si>
+  <si>
+    <t>Columns in Excel</t>
+  </si>
+  <si>
     <t>Cell in Excel</t>
   </si>
   <si>
+    <t>Columns in JSON</t>
+  </si>
+  <si>
+    <t>PercentageSmokers</t>
+  </si>
+  <si>
+    <t>FoodEnvironmentIndex</t>
+  </si>
+  <si>
+    <t>DrivingDeaths</t>
+  </si>
+  <si>
+    <t>MedicareEnrollees</t>
+  </si>
+  <si>
+    <t>PrimaryCarePhysicians</t>
+  </si>
+  <si>
+    <t>GraduationRate</t>
+  </si>
+  <si>
+    <t>PercentageUnemployed</t>
+  </si>
+  <si>
+    <t>TopPercentileIncome</t>
+  </si>
+  <si>
+    <t>AirPollution</t>
+  </si>
+  <si>
+    <t>WaterViolations</t>
+  </si>
+  <si>
+    <t>HouseholdProblems</t>
+  </si>
+  <si>
     <t>Comments / Discriptions</t>
   </si>
   <si>
-    <t>Quality of Life</t>
-  </si>
-  <si>
-    <t>Column Name</t>
+    <t>FIPS</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>County</t>
   </si>
   <si>
     <t>Z-Score</t>
@@ -118,47 +281,42 @@
     <t>Rank</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Load Z score</t>
-  </si>
-  <si>
-    <t>Load Rank</t>
+    <t>QualityofLife</t>
+  </si>
+  <si>
+    <t>EconomicFactors</t>
+  </si>
+  <si>
+    <t>ClinicalCare</t>
+  </si>
+  <si>
+    <t>HealthBehaviours</t>
+  </si>
+  <si>
+    <t>PhysicalEnvironment</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Cell Col Value</t>
+  </si>
+  <si>
+    <t>From file name</t>
+  </si>
+  <si>
+    <t>Col Level 1</t>
+  </si>
+  <si>
+    <t>Columns in Excel
+Col Level 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +327,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -195,7 +361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -222,6 +388,261 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -235,15 +656,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,162 +1013,538 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9052DD47-81F0-4B1C-A89F-DC6C9E9E735C}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="28"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="18"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="12">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="26"/>
+      <c r="B4" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="12">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="27"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="20">
+        <v>5</v>
+      </c>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="26"/>
+      <c r="B7" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="12">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="27"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="20">
+        <v>7</v>
+      </c>
+      <c r="D9" s="18"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="26"/>
+      <c r="B10" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="12">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="27"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="20">
+        <v>9</v>
+      </c>
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="26"/>
+      <c r="B13" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="12">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="27"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="20">
+        <v>11</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="26"/>
+      <c r="B16" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="12">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="20">
+        <v>0</v>
+      </c>
+      <c r="D18" s="18"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="12">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="12">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5E160C-BD6A-4FB2-9C78-E1B12AD86F87}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="11"/>
+      <c r="B2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="6">
         <v>27</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="2">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="11"/>
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="2">
+        <v>48</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="11"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="11"/>
+      <c r="B6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="2">
+        <v>62</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="2">
+        <v>79</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="11"/>
+      <c r="B8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="2">
+        <v>67</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="11"/>
+      <c r="B10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="2">
+        <v>101</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="2">
+        <v>111</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="11"/>
+      <c r="B12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="2">
+        <v>120</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="11"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="11"/>
+      <c r="B14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="2">
+        <v>141</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="2">
+        <v>144</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="11"/>
+      <c r="B16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="C16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="4">
+        <v>145</v>
+      </c>
+      <c r="G16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -720,7 +1552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286BFFA6-76A5-4566-B6F6-01830802E2EC}">
   <dimension ref="A2:F19"/>
   <sheetViews>
@@ -728,14 +1560,14 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -743,7 +1575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,7 +1586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -762,7 +1594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -773,17 +1605,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -797,7 +1629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>13</v>
       </c>
@@ -805,12 +1637,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>17</v>
       </c>
@@ -818,7 +1650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E19" t="s">
         <v>19</v>
       </c>

</xml_diff>